<commit_message>
Updating Search test cases
</commit_message>
<xml_diff>
--- a/testStrategy/test_cases.xlsx
+++ b/testStrategy/test_cases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="190">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -284,7 +284,56 @@
 4. Click search.</t>
   </si>
   <si>
-    <t xml:space="preserve">System displays a friendly 'no results found' message and may offer hints or suggestions; no technical errors.</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">System displays a friendly warning pop-up below the field after typing the non-existing route: “</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF3465A4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">We can’t find this place. Please check typos or try again with different keywords</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">”. If the “Search” button is pressed, then “</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Please choose an option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">” red text under the input field is shown</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Negative / Functional</t>
@@ -315,7 +364,7 @@
 4. Observe control behavior.</t>
   </si>
   <si>
-    <t xml:space="preserve">Control prevents exceeding the maximum (e.g., plus button disabled at limit or validation error is shown).</t>
+    <t xml:space="preserve">Control prevents exceeding the maximum by disabling the ‘+’ button</t>
   </si>
   <si>
     <t xml:space="preserve">Negative / Boundary</t>
@@ -691,26 +740,6 @@
   </si>
   <si>
     <t xml:space="preserve">Reliability / Security</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deep link with prefilled search parameters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Application supports URL parameters for origin, destination or date.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Open the booking URL with query parameters predefining origin, destination and date.
-2. Observe search form values.
-3. Trigger search without changing parameters.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search form initializes with values from URL parameters and search runs successfully, returning appropriate results.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Functional / Integration</t>
   </si>
 </sst>
 </file>
@@ -720,7 +749,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -747,6 +776,20 @@
       <b val="true"/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3465A4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -839,6 +882,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF3465A4"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1022,10 +1125,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1413,7 +1516,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="240.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
@@ -1439,7 +1542,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
@@ -1465,7 +1568,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="79.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
@@ -2121,32 +2224,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Test Cases: adding status column
</commit_message>
<xml_diff>
--- a/testStrategy/test_cases.xlsx
+++ b/testStrategy/test_cases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="189">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status</t>
   </si>
   <si>
     <t xml:space="preserve">Search</t>
@@ -75,6 +78,9 @@
     <t xml:space="preserve">Positive / Functional</t>
   </si>
   <si>
+    <t xml:space="preserve">Automated</t>
+  </si>
+  <si>
     <t xml:space="preserve">Successful return trip search</t>
   </si>
   <si>
@@ -89,6 +95,9 @@
   </si>
   <si>
     <t xml:space="preserve">Applicable only if return-trip option is supported in UI.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manual</t>
   </si>
   <si>
     <t xml:space="preserve">Swap ‘From’ and ‘To’ using swap control</t>
@@ -887,7 +896,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -902,6 +911,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1168,10 +1181,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1048576"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J40" activeCellId="0" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1184,35 +1197,39 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="18.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="16.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="21.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="14.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1220,25 +1237,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1246,28 +1266,31 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="I3" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1275,28 +1298,31 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1304,25 +1330,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1330,25 +1359,28 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1356,25 +1388,28 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1382,25 +1417,28 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1408,25 +1446,28 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1434,25 +1475,28 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1460,25 +1504,28 @@
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1486,25 +1533,28 @@
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1512,25 +1562,28 @@
         <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="240.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1538,25 +1591,28 @@
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1564,25 +1620,28 @@
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="79.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1590,25 +1649,28 @@
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="E16" s="3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>75</v>
+        <v>78</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1616,25 +1678,28 @@
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1642,25 +1707,28 @@
         <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1668,28 +1736,31 @@
         <v>19</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1697,25 +1768,28 @@
         <v>20</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1723,25 +1797,28 @@
         <v>21</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1749,25 +1826,28 @@
         <v>22</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1775,25 +1855,28 @@
         <v>23</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1801,25 +1884,28 @@
         <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1827,25 +1913,28 @@
         <v>25</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1853,25 +1942,28 @@
         <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1879,25 +1971,28 @@
         <v>27</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1905,25 +2000,28 @@
         <v>28</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="E28" s="3" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1931,25 +2029,28 @@
         <v>29</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1957,25 +2058,28 @@
         <v>30</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1983,25 +2087,28 @@
         <v>31</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2009,25 +2116,28 @@
         <v>32</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2035,25 +2145,28 @@
         <v>33</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2061,28 +2174,31 @@
         <v>34</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>152</v>
+        <v>155</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,25 +2206,28 @@
         <v>35</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2116,25 +2235,28 @@
         <v>36</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>162</v>
+        <v>165</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2142,25 +2264,29 @@
         <v>37</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
+      </c>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2168,25 +2294,28 @@
         <v>38</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>173</v>
+        <v>176</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2194,25 +2323,28 @@
         <v>39</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2220,29 +2352,30 @@
         <v>40</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>188</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
test_cases.xlsx: updating test cases
</commit_message>
<xml_diff>
--- a/testStrategy/test_cases.xlsx
+++ b/testStrategy/test_cases.xlsx
@@ -791,12 +791,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEE6EF"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -840,7 +846,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -857,16 +863,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -899,7 +901,7 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFDEE6EF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -1123,56 +1125,56 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="J23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="26.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="10.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="27.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="18.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="35.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="25.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="16.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="21.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.83"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Fixing: Identifier 'searchPage' has already been declared. (249:8)
</commit_message>
<xml_diff>
--- a/testStrategy/test_cases.xlsx
+++ b/testStrategy/test_cases.xlsx
@@ -1125,8 +1125,8 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J28" activeCellId="0" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1203,7 +1203,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="240.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="165.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>25</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>26</v>
       </c>
@@ -1934,10 +1934,10 @@
         <v>43</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>27</v>
       </c>
@@ -1963,10 +1963,10 @@
         <v>43</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>29</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>30</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>31</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>33</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <v>34</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
         <v>35</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
         <v>36</v>
       </c>

</xml_diff>